<commit_message>
Push spain hospital admission data
</commit_message>
<xml_diff>
--- a/data/hospitalisation_data/hospital_data_europe.xlsx
+++ b/data/hospitalisation_data/hospital_data_europe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\data\hospitalisation_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A31815-DC97-472C-B804-EEA1A50C0C31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44426F67-6A86-4D6D-BAFC-01351386D73A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>data</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>united-kingdom_hospital_admission</t>
+  </si>
+  <si>
+    <t>spain_hospital_admission</t>
   </si>
 </sst>
 </file>
@@ -189,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,6 +384,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -542,11 +557,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,26 +919,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I212"/>
+  <dimension ref="A1:J212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.36328125" customWidth="1"/>
     <col min="3" max="3" width="25.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.08984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32.81640625" customWidth="1"/>
-    <col min="9" max="9" width="32.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="32.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -943,14 +961,17 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -958,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43832</v>
       </c>
@@ -966,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>43833</v>
       </c>
@@ -974,7 +995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>43834</v>
       </c>
@@ -982,7 +1003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>43835</v>
       </c>
@@ -990,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>43836</v>
       </c>
@@ -998,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>43837</v>
       </c>
@@ -1006,7 +1027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43838</v>
       </c>
@@ -1014,7 +1035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>43839</v>
       </c>
@@ -1022,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>43840</v>
       </c>
@@ -1030,7 +1051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>43841</v>
       </c>
@@ -1038,7 +1059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>43842</v>
       </c>
@@ -1046,7 +1067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>43843</v>
       </c>
@@ -1054,7 +1075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>43844</v>
       </c>
@@ -1062,7 +1083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>43845</v>
       </c>
@@ -1454,7 +1475,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>43894</v>
       </c>
@@ -1462,7 +1483,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43895</v>
       </c>
@@ -1470,7 +1491,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>43896</v>
       </c>
@@ -1478,7 +1499,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>43897</v>
       </c>
@@ -1486,7 +1507,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>43898</v>
       </c>
@@ -1494,7 +1515,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>43899</v>
       </c>
@@ -1502,47 +1523,62 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>43900</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J71" s="5">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>43901</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J72" s="5">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>43902</v>
       </c>
       <c r="B73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J73" s="5">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>43903</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J74" s="5">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>43904</v>
       </c>
       <c r="B75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J75" s="5">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>43905</v>
       </c>
@@ -1558,8 +1594,11 @@
       <c r="E76" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J76" s="5">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>43906</v>
       </c>
@@ -1575,8 +1614,11 @@
       <c r="E77" s="2">
         <v>79</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J77" s="5">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>43907</v>
       </c>
@@ -1592,8 +1634,11 @@
       <c r="E78" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J78" s="5">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>43908</v>
       </c>
@@ -1612,8 +1657,11 @@
       <c r="F79" s="3">
         <v>2972</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J79" s="5">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>43909</v>
       </c>
@@ -1635,8 +1683,11 @@
       <c r="G80" s="3">
         <v>2229</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J80" s="5">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>43910</v>
       </c>
@@ -1658,8 +1709,11 @@
       <c r="G81" s="3">
         <v>1256</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J81" s="5">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>43911</v>
       </c>
@@ -1681,8 +1735,11 @@
       <c r="G82" s="3">
         <v>1540</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J82" s="5">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>43912</v>
       </c>
@@ -1704,8 +1761,11 @@
       <c r="G83" s="3">
         <v>1534</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J83" s="5">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>43913</v>
       </c>
@@ -1727,11 +1787,14 @@
       <c r="G84" s="3">
         <v>2053</v>
       </c>
-      <c r="I84">
+      <c r="I84" s="4">
         <v>1687</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J84" s="5">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>43914</v>
       </c>
@@ -1753,11 +1816,14 @@
       <c r="G85" s="3">
         <v>2618</v>
       </c>
-      <c r="I85">
+      <c r="I85" s="4">
         <v>1931</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J85" s="5">
+        <v>4241</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>43915</v>
       </c>
@@ -1779,11 +1845,14 @@
       <c r="G86" s="3">
         <v>3166</v>
       </c>
-      <c r="I86">
+      <c r="I86" s="4">
         <v>1969</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J86" s="5">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>43916</v>
       </c>
@@ -1805,11 +1874,14 @@
       <c r="G87" s="3">
         <v>3097</v>
       </c>
-      <c r="I87">
+      <c r="I87" s="4">
         <v>2222</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J87" s="5">
+        <v>5751</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>43917</v>
       </c>
@@ -1831,14 +1903,17 @@
       <c r="G88" s="3">
         <v>3059</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="4">
         <v>7044</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="4">
         <v>2165</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J88" s="5">
+        <v>5987</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>43918</v>
       </c>
@@ -1860,14 +1935,17 @@
       <c r="G89" s="3">
         <v>3353</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="4">
         <v>8020</v>
       </c>
-      <c r="I89">
+      <c r="I89" s="4">
         <v>2506</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J89" s="5">
+        <v>4976</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>43919</v>
       </c>
@@ -1889,14 +1967,17 @@
       <c r="G90" s="3">
         <v>2685</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="4">
         <v>9238</v>
       </c>
-      <c r="I90">
+      <c r="I90" s="4">
         <v>3121</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J90" s="5">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>43920</v>
       </c>
@@ -1918,14 +1999,17 @@
       <c r="G91" s="3">
         <v>3108</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="4">
         <v>10732</v>
       </c>
-      <c r="I91">
+      <c r="I91" s="4">
         <v>2817</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J91" s="5">
+        <v>3466</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>43921</v>
       </c>
@@ -1947,14 +2031,17 @@
       <c r="G92" s="3">
         <v>4146</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="4">
         <v>12204</v>
       </c>
-      <c r="I92">
+      <c r="I92" s="4">
         <v>3483</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J92" s="5">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>43922</v>
       </c>
@@ -1976,14 +2063,17 @@
       <c r="G93" s="3">
         <v>4281</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="4">
         <v>13111</v>
       </c>
-      <c r="I93">
+      <c r="I93" s="4">
         <v>3396</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J93" s="5">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>43923</v>
       </c>
@@ -2005,14 +2095,17 @@
       <c r="G94" s="3">
         <v>3845</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="4">
         <v>13265</v>
       </c>
-      <c r="I94">
+      <c r="I94" s="4">
         <v>2914</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J94" s="5">
+        <v>3834</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>43924</v>
       </c>
@@ -2034,14 +2127,17 @@
       <c r="G95" s="3">
         <v>3627</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="4">
         <v>14748</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="4">
         <v>2959</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J95" s="5">
+        <v>3834</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>43925</v>
       </c>
@@ -2063,14 +2159,17 @@
       <c r="G96" s="3">
         <v>2822</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="4">
         <v>16606</v>
       </c>
-      <c r="I96">
+      <c r="I96" s="4">
         <v>2918</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J96" s="5">
+        <v>2928</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>43926</v>
       </c>
@@ -2092,14 +2191,17 @@
       <c r="G97" s="3">
         <v>1931</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="4">
         <v>17801</v>
       </c>
-      <c r="I97">
+      <c r="I97" s="4">
         <v>3000</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J97" s="5">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>43927</v>
       </c>
@@ -2121,14 +2223,17 @@
       <c r="G98" s="3">
         <v>2754</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="4">
         <v>18280</v>
       </c>
-      <c r="I98">
+      <c r="I98" s="4">
         <v>3111</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J98" s="5">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>43928</v>
       </c>
@@ -2150,14 +2255,17 @@
       <c r="G99" s="3">
         <v>3277</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="4">
         <v>18980</v>
       </c>
-      <c r="I99">
+      <c r="I99" s="4">
         <v>3025</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J99" s="5">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>43929</v>
       </c>
@@ -2179,14 +2287,17 @@
       <c r="G100" s="3">
         <v>3139</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="4">
         <v>19361</v>
       </c>
-      <c r="I100">
+      <c r="I100" s="4">
         <v>2684</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J100" s="5">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>43930</v>
       </c>
@@ -2208,14 +2319,17 @@
       <c r="G101" s="3">
         <v>2990</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="4">
         <v>19524</v>
       </c>
-      <c r="I101">
+      <c r="I101" s="4">
         <v>2486</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J101" s="5">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>43931</v>
       </c>
@@ -2237,14 +2351,17 @@
       <c r="G102" s="3">
         <v>3161</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="4">
         <v>19648</v>
       </c>
-      <c r="I102">
+      <c r="I102" s="4">
         <v>2219</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J102" s="5">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>43932</v>
       </c>
@@ -2266,14 +2383,17 @@
       <c r="G103" s="3">
         <v>2044</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="4">
         <v>19518</v>
       </c>
-      <c r="I103">
+      <c r="I103" s="4">
         <v>1996</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J103" s="5">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>43933</v>
       </c>
@@ -2295,14 +2415,17 @@
       <c r="G104" s="3">
         <v>1688</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="4">
         <v>19872</v>
       </c>
-      <c r="I104">
+      <c r="I104" s="4">
         <v>2188</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J104" s="5">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>43934</v>
       </c>
@@ -2324,14 +2447,17 @@
       <c r="G105" s="3">
         <v>1257</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="4">
         <v>19397</v>
       </c>
-      <c r="I105">
+      <c r="I105" s="4">
         <v>2109</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J105" s="5">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>43935</v>
       </c>
@@ -2353,14 +2479,17 @@
       <c r="G106" s="3">
         <v>1965</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="4">
         <v>19257</v>
       </c>
-      <c r="I106">
+      <c r="I106" s="4">
         <v>1837</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J106" s="5">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>43936</v>
       </c>
@@ -2382,14 +2511,17 @@
       <c r="G107" s="3">
         <v>2415</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="4">
         <v>18552</v>
       </c>
-      <c r="I107">
+      <c r="I107" s="4">
         <v>2047</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J107" s="5">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>43937</v>
       </c>
@@ -2411,14 +2543,17 @@
       <c r="G108" s="3">
         <v>2084</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="4">
         <v>18277</v>
       </c>
-      <c r="I108">
+      <c r="I108" s="4">
         <v>1906</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J108" s="5">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>43938</v>
       </c>
@@ -2440,14 +2575,17 @@
       <c r="G109" s="3">
         <v>2166</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="4">
         <v>17320</v>
       </c>
-      <c r="I109">
+      <c r="I109" s="4">
         <v>1702</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J109" s="5">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>43939</v>
       </c>
@@ -2469,14 +2607,17 @@
       <c r="G110" s="3">
         <v>1565</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="4">
         <v>17462</v>
       </c>
-      <c r="I110">
+      <c r="I110" s="4">
         <v>1693</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J110" s="5">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>43940</v>
       </c>
@@ -2498,14 +2639,17 @@
       <c r="G111" s="3">
         <v>890</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="4">
         <v>17476</v>
       </c>
-      <c r="I111">
+      <c r="I111" s="4">
         <v>1704</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J111" s="5">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>43941</v>
       </c>
@@ -2527,14 +2671,17 @@
       <c r="G112" s="3">
         <v>1464</v>
       </c>
-      <c r="H112">
+      <c r="H112" s="4">
         <v>17356</v>
       </c>
-      <c r="I112">
+      <c r="I112" s="4">
         <v>1708</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J112" s="5">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>43942</v>
       </c>
@@ -2556,14 +2703,17 @@
       <c r="G113" s="3">
         <v>1885</v>
       </c>
-      <c r="H113">
+      <c r="H113" s="4">
         <v>17098</v>
       </c>
-      <c r="I113">
+      <c r="I113" s="4">
         <v>1527</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J113" s="5">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>43943</v>
       </c>
@@ -2585,14 +2735,17 @@
       <c r="G114" s="3">
         <v>1619</v>
       </c>
-      <c r="H114">
+      <c r="H114" s="4">
         <v>16522</v>
       </c>
-      <c r="I114">
+      <c r="I114" s="4">
         <v>1504</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J114" s="5">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>43944</v>
       </c>
@@ -2614,14 +2767,17 @@
       <c r="G115" s="3">
         <v>1410</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="4">
         <v>15957</v>
       </c>
-      <c r="I115">
+      <c r="I115" s="4">
         <v>1500</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J115" s="5">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>43945</v>
       </c>
@@ -2643,14 +2799,17 @@
       <c r="G116" s="3">
         <v>1346</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="4">
         <v>15339</v>
       </c>
-      <c r="I116">
+      <c r="I116" s="4">
         <v>1329</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J116" s="5">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>43946</v>
       </c>
@@ -2672,14 +2831,17 @@
       <c r="G117" s="3">
         <v>999</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="4">
         <v>14799</v>
       </c>
-      <c r="I117">
+      <c r="I117" s="4">
         <v>1380</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J117" s="5">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>43947</v>
       </c>
@@ -2701,14 +2863,17 @@
       <c r="G118" s="3">
         <v>481</v>
       </c>
-      <c r="H118">
+      <c r="H118" s="4">
         <v>14695</v>
       </c>
-      <c r="I118">
+      <c r="I118" s="4">
         <v>1491</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J118" s="5">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>43948</v>
       </c>
@@ -2730,14 +2895,17 @@
       <c r="G119" s="3">
         <v>964</v>
       </c>
-      <c r="H119">
+      <c r="H119" s="4">
         <v>14788</v>
       </c>
-      <c r="I119">
+      <c r="I119" s="4">
         <v>1487</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J119" s="5">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>43949</v>
       </c>
@@ -2759,14 +2927,17 @@
       <c r="G120" s="3">
         <v>1321</v>
       </c>
-      <c r="H120">
+      <c r="H120" s="4">
         <v>14113</v>
       </c>
-      <c r="I120">
+      <c r="I120" s="4">
         <v>1516</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J120" s="5">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>43950</v>
       </c>
@@ -2788,14 +2959,17 @@
       <c r="G121" s="3">
         <v>1070</v>
       </c>
-      <c r="H121">
+      <c r="H121" s="4">
         <v>13851</v>
       </c>
-      <c r="I121">
+      <c r="I121" s="4">
         <v>1417</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J121" s="5">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>43951</v>
       </c>
@@ -2817,14 +2991,17 @@
       <c r="G122" s="3">
         <v>1048</v>
       </c>
-      <c r="H122">
+      <c r="H122" s="4">
         <v>13475</v>
       </c>
-      <c r="I122">
+      <c r="I122" s="4">
         <v>1297</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J122" s="5">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>43952</v>
       </c>
@@ -2846,14 +3023,17 @@
       <c r="G123" s="3">
         <v>668</v>
       </c>
-      <c r="H123">
+      <c r="H123" s="4">
         <v>13051</v>
       </c>
-      <c r="I123">
+      <c r="I123" s="4">
         <v>1162</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J123" s="5">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>43953</v>
       </c>
@@ -2875,14 +3055,17 @@
       <c r="G124" s="3">
         <v>453</v>
       </c>
-      <c r="H124">
+      <c r="H124" s="4">
         <v>12766</v>
       </c>
-      <c r="I124">
+      <c r="I124" s="4">
         <v>1242</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J124" s="5">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>43954</v>
       </c>
@@ -2904,14 +3087,17 @@
       <c r="G125" s="3">
         <v>345</v>
       </c>
-      <c r="H125">
+      <c r="H125" s="4">
         <v>12607</v>
       </c>
-      <c r="I125">
+      <c r="I125" s="4">
         <v>1206</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J125" s="5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>43955</v>
       </c>
@@ -2933,14 +3119,17 @@
       <c r="G126" s="3">
         <v>689</v>
       </c>
-      <c r="H126">
+      <c r="H126" s="4">
         <v>12493</v>
       </c>
-      <c r="I126">
+      <c r="I126" s="4">
         <v>1143</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J126" s="5">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>43956</v>
       </c>
@@ -2962,14 +3151,17 @@
       <c r="G127" s="3">
         <v>987</v>
       </c>
-      <c r="H127">
+      <c r="H127" s="4">
         <v>12152</v>
       </c>
-      <c r="I127">
+      <c r="I127" s="4">
         <v>1226</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J127" s="5">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>43957</v>
       </c>
@@ -2991,14 +3183,17 @@
       <c r="G128" s="3">
         <v>833</v>
       </c>
-      <c r="H128">
+      <c r="H128" s="4">
         <v>11682</v>
       </c>
-      <c r="I128">
+      <c r="I128" s="4">
         <v>1162</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J128" s="5">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>43958</v>
       </c>
@@ -3020,14 +3215,17 @@
       <c r="G129" s="3">
         <v>728</v>
       </c>
-      <c r="H129">
+      <c r="H129" s="4">
         <v>11161</v>
       </c>
-      <c r="I129">
+      <c r="I129" s="4">
         <v>909</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J129" s="5">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>43959</v>
       </c>
@@ -3049,14 +3247,17 @@
       <c r="G130" s="3">
         <v>510</v>
       </c>
-      <c r="H130">
+      <c r="H130" s="4">
         <v>10689</v>
       </c>
-      <c r="I130">
+      <c r="I130" s="4">
         <v>964</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J130" s="5">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>43960</v>
       </c>
@@ -3078,14 +3279,17 @@
       <c r="G131" s="3">
         <v>265</v>
       </c>
-      <c r="H131">
+      <c r="H131" s="4">
         <v>10701</v>
       </c>
-      <c r="I131">
+      <c r="I131" s="4">
         <v>899</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J131" s="5">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>43961</v>
       </c>
@@ -3107,14 +3311,17 @@
       <c r="G132" s="3">
         <v>253</v>
       </c>
-      <c r="H132">
+      <c r="H132" s="4">
         <v>10432</v>
       </c>
-      <c r="I132">
+      <c r="I132" s="4">
         <v>1025</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J132" s="5">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>43962</v>
       </c>
@@ -3136,14 +3343,17 @@
       <c r="G133" s="3">
         <v>523</v>
       </c>
-      <c r="H133">
+      <c r="H133" s="4">
         <v>10659</v>
       </c>
-      <c r="I133">
+      <c r="I133" s="4">
         <v>1006</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J133" s="5">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>43963</v>
       </c>
@@ -3165,14 +3375,17 @@
       <c r="G134" s="3">
         <v>670</v>
       </c>
-      <c r="H134">
+      <c r="H134" s="4">
         <v>10343</v>
       </c>
-      <c r="I134">
+      <c r="I134" s="4">
         <v>943</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J134" s="5">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>43964</v>
       </c>
@@ -3194,14 +3407,17 @@
       <c r="G135" s="3">
         <v>543</v>
       </c>
-      <c r="H135">
+      <c r="H135" s="4">
         <v>10088</v>
       </c>
-      <c r="I135">
+      <c r="I135" s="4">
         <v>925</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J135" s="5">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>43965</v>
       </c>
@@ -3223,14 +3439,17 @@
       <c r="G136" s="3">
         <v>542</v>
       </c>
-      <c r="H136">
+      <c r="H136" s="4">
         <v>9702</v>
       </c>
-      <c r="I136">
+      <c r="I136" s="4">
         <v>882</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J136" s="5">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>43966</v>
       </c>
@@ -3252,14 +3471,17 @@
       <c r="G137" s="3">
         <v>438</v>
       </c>
-      <c r="H137">
+      <c r="H137" s="4">
         <v>9497</v>
       </c>
-      <c r="I137">
+      <c r="I137" s="4">
         <v>801</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J137" s="5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>43967</v>
       </c>
@@ -3281,14 +3503,17 @@
       <c r="G138" s="3">
         <v>350</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="4">
         <v>9105</v>
       </c>
-      <c r="I138">
+      <c r="I138" s="4">
         <v>816</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J138" s="5">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>43968</v>
       </c>
@@ -3310,14 +3535,17 @@
       <c r="G139" s="3">
         <v>152</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="4">
         <v>9124</v>
       </c>
-      <c r="I139">
+      <c r="I139" s="4">
         <v>852</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J139" s="5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>43969</v>
       </c>
@@ -3339,14 +3567,17 @@
       <c r="G140" s="3">
         <v>375</v>
       </c>
-      <c r="H140">
+      <c r="H140" s="4">
         <v>9095</v>
       </c>
-      <c r="I140">
+      <c r="I140" s="4">
         <v>866</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J140" s="5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>43970</v>
       </c>
@@ -3368,14 +3599,17 @@
       <c r="G141" s="3">
         <v>506</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="4">
         <v>8914</v>
       </c>
-      <c r="I141">
+      <c r="I141" s="4">
         <v>859</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J141" s="5">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>43971</v>
       </c>
@@ -3397,14 +3631,17 @@
       <c r="G142" s="3">
         <v>432</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="4">
         <v>8512</v>
       </c>
-      <c r="I142">
+      <c r="I142" s="4">
         <v>832</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J142" s="5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>43972</v>
       </c>
@@ -3426,14 +3663,17 @@
       <c r="G143" s="3">
         <v>271</v>
       </c>
-      <c r="H143">
+      <c r="H143" s="4">
         <v>8268</v>
       </c>
-      <c r="I143">
+      <c r="I143" s="4">
         <v>764</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J143" s="5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>43973</v>
       </c>
@@ -3455,14 +3695,17 @@
       <c r="G144" s="3">
         <v>263</v>
       </c>
-      <c r="H144">
+      <c r="H144" s="4">
         <v>8233</v>
       </c>
-      <c r="I144">
+      <c r="I144" s="4">
         <v>605</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J144" s="5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>43974</v>
       </c>
@@ -3484,14 +3727,17 @@
       <c r="G145" s="3">
         <v>233</v>
       </c>
-      <c r="H145">
+      <c r="H145" s="4">
         <v>7867</v>
       </c>
-      <c r="I145">
+      <c r="I145" s="4">
         <v>635</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J145" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>43975</v>
       </c>
@@ -3513,14 +3759,14 @@
       <c r="G146" s="3">
         <v>121</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="4">
         <v>7871</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="4">
         <v>589</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>43976</v>
       </c>
@@ -3542,14 +3788,14 @@
       <c r="G147" s="3">
         <v>342</v>
       </c>
-      <c r="H147">
+      <c r="H147" s="4">
         <v>7895</v>
       </c>
-      <c r="I147">
+      <c r="I147" s="4">
         <v>683</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>43977</v>
       </c>
@@ -3571,14 +3817,14 @@
       <c r="G148" s="3">
         <v>318</v>
       </c>
-      <c r="H148">
+      <c r="H148" s="4">
         <v>7800</v>
       </c>
-      <c r="I148">
+      <c r="I148" s="4">
         <v>707</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>43978</v>
       </c>
@@ -3600,14 +3846,14 @@
       <c r="G149" s="3">
         <v>271</v>
       </c>
-      <c r="H149">
+      <c r="H149" s="4">
         <v>7474</v>
       </c>
-      <c r="I149">
+      <c r="I149" s="4">
         <v>691</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>43979</v>
       </c>
@@ -3629,14 +3875,14 @@
       <c r="G150" s="3">
         <v>253</v>
       </c>
-      <c r="H150">
+      <c r="H150" s="4">
         <v>7211</v>
       </c>
-      <c r="I150">
+      <c r="I150" s="4">
         <v>631</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>43980</v>
       </c>
@@ -3658,14 +3904,14 @@
       <c r="G151" s="3">
         <v>255</v>
       </c>
-      <c r="H151">
+      <c r="H151" s="4">
         <v>6909</v>
       </c>
-      <c r="I151">
+      <c r="I151" s="4">
         <v>580</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>43981</v>
       </c>
@@ -3687,14 +3933,14 @@
       <c r="G152" s="3">
         <v>227</v>
       </c>
-      <c r="H152">
+      <c r="H152" s="4">
         <v>6619</v>
       </c>
-      <c r="I152">
+      <c r="I152" s="4">
         <v>548</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>43982</v>
       </c>
@@ -3716,14 +3962,14 @@
       <c r="G153" s="3">
         <v>72</v>
       </c>
-      <c r="H153">
+      <c r="H153" s="4">
         <v>6587</v>
       </c>
-      <c r="I153">
+      <c r="I153" s="4">
         <v>604</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>43983</v>
       </c>
@@ -3745,14 +3991,14 @@
       <c r="G154" s="3">
         <v>89</v>
       </c>
-      <c r="H154">
+      <c r="H154" s="4">
         <v>6635</v>
       </c>
-      <c r="I154">
+      <c r="I154" s="4">
         <v>635</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>43984</v>
       </c>
@@ -3774,14 +4020,14 @@
       <c r="G155" s="3">
         <v>229</v>
       </c>
-      <c r="H155">
+      <c r="H155" s="4">
         <v>6451</v>
       </c>
-      <c r="I155">
+      <c r="I155" s="4">
         <v>605</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>43985</v>
       </c>
@@ -3803,14 +4049,14 @@
       <c r="G156" s="3">
         <v>250</v>
       </c>
-      <c r="H156">
+      <c r="H156" s="4">
         <v>6254</v>
       </c>
-      <c r="I156">
+      <c r="I156" s="4">
         <v>599</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>43986</v>
       </c>
@@ -3832,14 +4078,14 @@
       <c r="G157" s="3">
         <v>195</v>
       </c>
-      <c r="H157">
+      <c r="H157" s="4">
         <v>5996</v>
       </c>
-      <c r="I157">
+      <c r="I157" s="4">
         <v>486</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>43987</v>
       </c>
@@ -3861,14 +4107,14 @@
       <c r="G158" s="3">
         <v>213</v>
       </c>
-      <c r="H158">
+      <c r="H158" s="4">
         <v>5841</v>
       </c>
-      <c r="I158">
+      <c r="I158" s="4">
         <v>400</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>43988</v>
       </c>
@@ -3890,14 +4136,14 @@
       <c r="G159" s="3">
         <v>143</v>
       </c>
-      <c r="H159">
+      <c r="H159" s="4">
         <v>5631</v>
       </c>
-      <c r="I159">
+      <c r="I159" s="4">
         <v>423</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>43989</v>
       </c>
@@ -3919,10 +4165,10 @@
       <c r="G160" s="3">
         <v>37</v>
       </c>
-      <c r="H160">
+      <c r="H160" s="4">
         <v>5430</v>
       </c>
-      <c r="I160">
+      <c r="I160" s="4">
         <v>431</v>
       </c>
     </row>
@@ -3948,10 +4194,10 @@
       <c r="G161" s="3">
         <v>145</v>
       </c>
-      <c r="H161">
+      <c r="H161" s="4">
         <v>5409</v>
       </c>
-      <c r="I161">
+      <c r="I161" s="4">
         <v>461</v>
       </c>
     </row>
@@ -3977,10 +4223,10 @@
       <c r="G162" s="3">
         <v>169</v>
       </c>
-      <c r="H162">
+      <c r="H162" s="4">
         <v>5230</v>
       </c>
-      <c r="I162">
+      <c r="I162" s="4">
         <v>497</v>
       </c>
     </row>
@@ -4006,10 +4252,10 @@
       <c r="G163" s="3">
         <v>130</v>
       </c>
-      <c r="H163">
+      <c r="H163" s="4">
         <v>4972</v>
       </c>
-      <c r="I163">
+      <c r="I163" s="4">
         <v>440</v>
       </c>
     </row>
@@ -4035,10 +4281,10 @@
       <c r="G164" s="3">
         <v>143</v>
       </c>
-      <c r="H164">
+      <c r="H164" s="4">
         <v>4732</v>
       </c>
-      <c r="I164">
+      <c r="I164" s="4">
         <v>413</v>
       </c>
     </row>
@@ -4064,10 +4310,10 @@
       <c r="G165" s="3">
         <v>136</v>
       </c>
-      <c r="H165">
+      <c r="H165" s="4">
         <v>4662</v>
       </c>
-      <c r="I165">
+      <c r="I165" s="4">
         <v>358</v>
       </c>
     </row>
@@ -4093,10 +4339,10 @@
       <c r="G166" s="3">
         <v>68</v>
       </c>
-      <c r="H166">
+      <c r="H166" s="4">
         <v>4520</v>
       </c>
-      <c r="I166">
+      <c r="I166" s="4">
         <v>426</v>
       </c>
     </row>
@@ -4122,10 +4368,10 @@
       <c r="G167" s="3">
         <v>33</v>
       </c>
-      <c r="H167">
+      <c r="H167" s="4">
         <v>4519</v>
       </c>
-      <c r="I167">
+      <c r="I167" s="4">
         <v>423</v>
       </c>
     </row>
@@ -4151,10 +4397,10 @@
       <c r="G168" s="3">
         <v>114</v>
       </c>
-      <c r="H168">
+      <c r="H168" s="4">
         <v>4489</v>
       </c>
-      <c r="I168">
+      <c r="I168" s="4">
         <v>428</v>
       </c>
     </row>
@@ -4180,10 +4426,10 @@
       <c r="G169" s="3">
         <v>143</v>
       </c>
-      <c r="H169">
+      <c r="H169" s="4">
         <v>4490</v>
       </c>
-      <c r="I169">
+      <c r="I169" s="4">
         <v>434</v>
       </c>
     </row>
@@ -4209,10 +4455,10 @@
       <c r="G170" s="3">
         <v>116</v>
       </c>
-      <c r="H170">
+      <c r="H170" s="4">
         <v>4348</v>
       </c>
-      <c r="I170">
+      <c r="I170" s="4">
         <v>409</v>
       </c>
     </row>
@@ -4238,10 +4484,10 @@
       <c r="G171" s="3">
         <v>136</v>
       </c>
-      <c r="H171">
+      <c r="H171" s="4">
         <v>4217</v>
       </c>
-      <c r="I171">
+      <c r="I171" s="4">
         <v>342</v>
       </c>
     </row>
@@ -4267,10 +4513,10 @@
       <c r="G172" s="3">
         <v>116</v>
       </c>
-      <c r="H172">
+      <c r="H172" s="4">
         <v>4078</v>
       </c>
-      <c r="I172">
+      <c r="I172" s="4">
         <v>266</v>
       </c>
     </row>
@@ -4296,10 +4542,10 @@
       <c r="G173" s="3">
         <v>90</v>
       </c>
-      <c r="H173">
+      <c r="H173" s="4">
         <v>3926</v>
       </c>
-      <c r="I173">
+      <c r="I173" s="4">
         <v>288</v>
       </c>
     </row>
@@ -4325,10 +4571,10 @@
       <c r="G174" s="3">
         <v>48</v>
       </c>
-      <c r="H174">
+      <c r="H174" s="4">
         <v>3898</v>
       </c>
-      <c r="I174">
+      <c r="I174" s="4">
         <v>390</v>
       </c>
     </row>
@@ -4354,10 +4600,10 @@
       <c r="G175" s="3">
         <v>142</v>
       </c>
-      <c r="H175">
+      <c r="H175" s="4">
         <v>3961</v>
       </c>
-      <c r="I175">
+      <c r="I175" s="4">
         <v>347</v>
       </c>
     </row>
@@ -4383,10 +4629,10 @@
       <c r="G176" s="3">
         <v>117</v>
       </c>
-      <c r="H176">
+      <c r="H176" s="4">
         <v>3841</v>
       </c>
-      <c r="I176">
+      <c r="I176" s="4">
         <v>347</v>
       </c>
     </row>
@@ -4412,10 +4658,10 @@
       <c r="G177" s="3">
         <v>97</v>
       </c>
-      <c r="H177">
+      <c r="H177" s="4">
         <v>3731</v>
       </c>
-      <c r="I177">
+      <c r="I177" s="4">
         <v>361</v>
       </c>
     </row>
@@ -4441,10 +4687,10 @@
       <c r="G178" s="3">
         <v>124</v>
       </c>
-      <c r="H178">
+      <c r="H178" s="4">
         <v>3585</v>
       </c>
-      <c r="I178">
+      <c r="I178" s="4">
         <v>315</v>
       </c>
     </row>
@@ -4470,10 +4716,10 @@
       <c r="G179" s="3">
         <v>87</v>
       </c>
-      <c r="H179">
+      <c r="H179" s="4">
         <v>3362</v>
       </c>
-      <c r="I179">
+      <c r="I179" s="4">
         <v>298</v>
       </c>
     </row>
@@ -4499,10 +4745,10 @@
       <c r="G180" s="3">
         <v>55</v>
       </c>
-      <c r="H180">
+      <c r="H180" s="4">
         <v>3285</v>
       </c>
-      <c r="I180">
+      <c r="I180" s="4">
         <v>231</v>
       </c>
     </row>
@@ -4528,10 +4774,10 @@
       <c r="G181" s="3">
         <v>44</v>
       </c>
-      <c r="H181">
+      <c r="H181" s="4">
         <v>3309</v>
       </c>
-      <c r="I181">
+      <c r="I181" s="4">
         <v>224</v>
       </c>
     </row>
@@ -4557,10 +4803,10 @@
       <c r="G182" s="3">
         <v>102</v>
       </c>
-      <c r="H182">
+      <c r="H182" s="4">
         <v>3491</v>
       </c>
-      <c r="I182">
+      <c r="I182" s="4">
         <v>237</v>
       </c>
     </row>
@@ -4586,10 +4832,10 @@
       <c r="G183" s="3">
         <v>152</v>
       </c>
-      <c r="H183">
+      <c r="H183" s="4">
         <v>3145</v>
       </c>
-      <c r="I183">
+      <c r="I183" s="4">
         <v>306</v>
       </c>
     </row>
@@ -4615,10 +4861,10 @@
       <c r="G184" s="3">
         <v>106</v>
       </c>
-      <c r="H184">
+      <c r="H184" s="4">
         <v>2964</v>
       </c>
-      <c r="I184">
+      <c r="I184" s="4">
         <v>217</v>
       </c>
     </row>
@@ -4644,10 +4890,10 @@
       <c r="G185" s="3">
         <v>93</v>
       </c>
-      <c r="H185">
+      <c r="H185" s="4">
         <v>2843</v>
       </c>
-      <c r="I185">
+      <c r="I185" s="4">
         <v>210</v>
       </c>
     </row>
@@ -4673,10 +4919,10 @@
       <c r="G186" s="3">
         <v>125</v>
       </c>
-      <c r="H186">
+      <c r="H186" s="4">
         <v>2721</v>
       </c>
-      <c r="I186">
+      <c r="I186" s="4">
         <v>187</v>
       </c>
     </row>
@@ -4702,10 +4948,10 @@
       <c r="G187" s="3">
         <v>47</v>
       </c>
-      <c r="H187">
+      <c r="H187" s="4">
         <v>2589</v>
       </c>
-      <c r="I187">
+      <c r="I187" s="4">
         <v>212</v>
       </c>
     </row>
@@ -4731,10 +4977,10 @@
       <c r="G188" s="3">
         <v>21</v>
       </c>
-      <c r="H188">
+      <c r="H188" s="4">
         <v>2550</v>
       </c>
-      <c r="I188">
+      <c r="I188" s="4">
         <v>215</v>
       </c>
     </row>
@@ -4760,10 +5006,10 @@
       <c r="G189" s="3">
         <v>98</v>
       </c>
-      <c r="H189">
+      <c r="H189" s="4">
         <v>2496</v>
       </c>
-      <c r="I189">
+      <c r="I189" s="4">
         <v>200</v>
       </c>
     </row>
@@ -4789,10 +5035,10 @@
       <c r="G190" s="3">
         <v>127</v>
       </c>
-      <c r="H190">
+      <c r="H190" s="4">
         <v>2393</v>
       </c>
-      <c r="I190">
+      <c r="I190" s="4">
         <v>206</v>
       </c>
     </row>
@@ -4818,10 +5064,10 @@
       <c r="G191" s="3">
         <v>83</v>
       </c>
-      <c r="H191">
+      <c r="H191" s="4">
         <v>2252</v>
       </c>
-      <c r="I191">
+      <c r="I191" s="4">
         <v>201</v>
       </c>
     </row>
@@ -4847,10 +5093,10 @@
       <c r="G192" s="3">
         <v>79</v>
       </c>
-      <c r="H192">
+      <c r="H192" s="4">
         <v>2173</v>
       </c>
-      <c r="I192">
+      <c r="I192" s="4">
         <v>179</v>
       </c>
     </row>
@@ -4876,10 +5122,10 @@
       <c r="G193" s="3">
         <v>136</v>
       </c>
-      <c r="H193">
+      <c r="H193" s="4">
         <v>2088</v>
       </c>
-      <c r="I193">
+      <c r="I193" s="4">
         <v>167</v>
       </c>
     </row>
@@ -4905,10 +5151,10 @@
       <c r="G194" s="3">
         <v>57</v>
       </c>
-      <c r="H194">
+      <c r="H194" s="4">
         <v>1940</v>
       </c>
-      <c r="I194">
+      <c r="I194" s="4">
         <v>150</v>
       </c>
     </row>
@@ -4934,10 +5180,10 @@
       <c r="G195" s="3">
         <v>26</v>
       </c>
-      <c r="H195">
+      <c r="H195" s="4">
         <v>1950</v>
       </c>
-      <c r="I195">
+      <c r="I195" s="4">
         <v>179</v>
       </c>
     </row>
@@ -4963,10 +5209,10 @@
       <c r="G196" s="3">
         <v>68</v>
       </c>
-      <c r="H196">
+      <c r="H196" s="4">
         <v>1959</v>
       </c>
-      <c r="I196">
+      <c r="I196" s="4">
         <v>173</v>
       </c>
     </row>
@@ -4992,10 +5238,10 @@
       <c r="G197" s="3">
         <v>61</v>
       </c>
-      <c r="H197">
+      <c r="H197" s="4">
         <v>1864</v>
       </c>
-      <c r="I197">
+      <c r="I197" s="4">
         <v>179</v>
       </c>
     </row>
@@ -5021,10 +5267,10 @@
       <c r="G198" s="3">
         <v>133</v>
       </c>
-      <c r="H198">
+      <c r="H198" s="4">
         <v>1834</v>
       </c>
-      <c r="I198">
+      <c r="I198" s="4">
         <v>163</v>
       </c>
     </row>
@@ -5050,7 +5296,7 @@
       <c r="G199" s="3">
         <v>119</v>
       </c>
-      <c r="H199">
+      <c r="H199" s="4">
         <v>1690</v>
       </c>
     </row>
@@ -5076,7 +5322,7 @@
       <c r="G200" s="3">
         <v>119</v>
       </c>
-      <c r="H200">
+      <c r="H200" s="4">
         <v>1676</v>
       </c>
     </row>
@@ -5102,7 +5348,7 @@
       <c r="G201" s="3">
         <v>68</v>
       </c>
-      <c r="H201">
+      <c r="H201" s="4">
         <v>1649</v>
       </c>
     </row>
@@ -5128,7 +5374,7 @@
       <c r="G202" s="3">
         <v>36</v>
       </c>
-      <c r="H202">
+      <c r="H202" s="4">
         <v>1613</v>
       </c>
     </row>
@@ -5154,7 +5400,7 @@
       <c r="G203" s="3">
         <v>137</v>
       </c>
-      <c r="H203">
+      <c r="H203" s="4">
         <v>1600</v>
       </c>
     </row>
@@ -5180,7 +5426,7 @@
       <c r="G204" s="3">
         <v>109</v>
       </c>
-      <c r="H204">
+      <c r="H204" s="4">
         <v>1510</v>
       </c>
     </row>
@@ -5206,7 +5452,7 @@
       <c r="G205" s="3">
         <v>132</v>
       </c>
-      <c r="H205">
+      <c r="H205" s="4">
         <v>1637</v>
       </c>
     </row>
@@ -5232,7 +5478,7 @@
       <c r="G206" s="3">
         <v>123</v>
       </c>
-      <c r="H206">
+      <c r="H206" s="4">
         <v>1445</v>
       </c>
     </row>
@@ -5258,7 +5504,7 @@
       <c r="G207" s="3">
         <v>126</v>
       </c>
-      <c r="H207">
+      <c r="H207" s="4">
         <v>1346</v>
       </c>
     </row>
@@ -5284,7 +5530,7 @@
       <c r="G208" s="3">
         <v>86</v>
       </c>
-      <c r="H208">
+      <c r="H208" s="4">
         <v>1257</v>
       </c>
     </row>
@@ -5310,7 +5556,7 @@
       <c r="G209" s="3">
         <v>36</v>
       </c>
-      <c r="H209">
+      <c r="H209" s="4">
         <v>1286</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Push hospital data for Italy
</commit_message>
<xml_diff>
--- a/data/hospitalisation_data/hospital_data_europe.xlsx
+++ b/data/hospitalisation_data/hospital_data_europe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\data\hospitalisation_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44426F67-6A86-4D6D-BAFC-01351386D73A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4865A293-F0E8-4910-ABE1-7455CF22C27D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
   <si>
     <t>data</t>
   </si>
@@ -51,12 +51,15 @@
   <si>
     <t>spain_hospital_admission</t>
   </si>
+  <si>
+    <t>italy_hospital_occupancy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +194,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +405,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -557,13 +572,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J212"/>
+  <dimension ref="A1:K212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I165" sqref="I165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -936,10 +952,11 @@
     <col min="7" max="7" width="24.08984375" style="3" customWidth="1"/>
     <col min="8" max="8" width="32.81640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="32.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -970,8 +987,11 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -979,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43832</v>
       </c>
@@ -987,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>43833</v>
       </c>
@@ -995,7 +1015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>43834</v>
       </c>
@@ -1003,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>43835</v>
       </c>
@@ -1011,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>43836</v>
       </c>
@@ -1019,7 +1039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>43837</v>
       </c>
@@ -1027,7 +1047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43838</v>
       </c>
@@ -1035,7 +1055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>43839</v>
       </c>
@@ -1043,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>43840</v>
       </c>
@@ -1051,7 +1071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>43841</v>
       </c>
@@ -1059,7 +1079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>43842</v>
       </c>
@@ -1067,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>43843</v>
       </c>
@@ -1075,7 +1095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>43844</v>
       </c>
@@ -1083,7 +1103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>43845</v>
       </c>
@@ -1347,7 +1367,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>43878</v>
       </c>
@@ -1355,7 +1375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43879</v>
       </c>
@@ -1363,7 +1383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>43880</v>
       </c>
@@ -1371,7 +1391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>43881</v>
       </c>
@@ -1379,7 +1399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>43882</v>
       </c>
@@ -1387,7 +1407,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43883</v>
       </c>
@@ -1395,7 +1415,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>43884</v>
       </c>
@@ -1403,127 +1423,172 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>43885</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K56" s="6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>43886</v>
       </c>
       <c r="B57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K57" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>43887</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K58" s="6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>43888</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K59" s="6">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>43889</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K60" s="6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>43890</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K61" s="6">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>43891</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K62" s="6">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>43892</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="K63" s="6">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>43893</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K64" s="6">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>43894</v>
       </c>
       <c r="B65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K65" s="6">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43895</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K66" s="6">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>43896</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K67" s="6">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>43897</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K68" s="6">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>43898</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K69" s="6">
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>43899</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K70" s="6">
+        <v>5049</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>43900</v>
       </c>
@@ -1533,8 +1598,11 @@
       <c r="J71" s="5">
         <v>1129</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K71" s="6">
+        <v>5915</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>43901</v>
       </c>
@@ -1544,8 +1612,11 @@
       <c r="J72" s="5">
         <v>460</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K72" s="6">
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>43902</v>
       </c>
@@ -1555,8 +1626,11 @@
       <c r="J73" s="5">
         <v>683</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K73" s="6">
+        <v>7803</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>43903</v>
       </c>
@@ -1566,8 +1640,11 @@
       <c r="J74" s="5">
         <v>643</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K74" s="6">
+        <v>8754</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>43904</v>
       </c>
@@ -1577,8 +1654,11 @@
       <c r="J75" s="5">
         <v>840</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K75" s="6">
+        <v>9890</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>43905</v>
       </c>
@@ -1597,8 +1677,11 @@
       <c r="J76" s="5">
         <v>1037</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K76" s="6">
+        <v>11335</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>43906</v>
       </c>
@@ -1617,8 +1700,11 @@
       <c r="J77" s="5">
         <v>1050</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K77" s="6">
+        <v>12876</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>43907</v>
       </c>
@@ -1637,8 +1723,11 @@
       <c r="J78" s="5">
         <v>1392</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K78" s="6">
+        <v>14954</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>43908</v>
       </c>
@@ -1660,8 +1749,11 @@
       <c r="J79" s="5">
         <v>1799</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K79" s="6">
+        <v>16620</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>43909</v>
       </c>
@@ -1686,8 +1778,11 @@
       <c r="J80" s="5">
         <v>2311</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K80" s="6">
+        <v>18255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>43910</v>
       </c>
@@ -1712,8 +1807,11 @@
       <c r="J81" s="5">
         <v>3125</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K81" s="6">
+        <v>18675</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>43911</v>
       </c>
@@ -1738,8 +1836,11 @@
       <c r="J82" s="5">
         <v>3046</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K82" s="6">
+        <v>20565</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>43912</v>
       </c>
@@ -1764,8 +1865,11 @@
       <c r="J83" s="5">
         <v>3335</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K83" s="6">
+        <v>22855</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>43913</v>
       </c>
@@ -1793,8 +1897,11 @@
       <c r="J84" s="5">
         <v>4070</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K84" s="6">
+        <v>23896</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>43914</v>
       </c>
@@ -1822,8 +1929,11 @@
       <c r="J85" s="5">
         <v>4241</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K85" s="6">
+        <v>25333</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>43915</v>
       </c>
@@ -1851,8 +1961,11 @@
       <c r="J86" s="5">
         <v>4950</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K86" s="6">
+        <v>26601</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>43916</v>
       </c>
@@ -1880,8 +1993,11 @@
       <c r="J87" s="5">
         <v>5751</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K87" s="6">
+        <v>28365</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>43917</v>
       </c>
@@ -1912,8 +2028,11 @@
       <c r="J88" s="5">
         <v>5987</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K88" s="6">
+        <v>29761</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>43918</v>
       </c>
@@ -1944,8 +2063,11 @@
       <c r="J89" s="5">
         <v>4976</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K89" s="6">
+        <v>30532</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>43919</v>
       </c>
@@ -1976,8 +2098,11 @@
       <c r="J90" s="5">
         <v>4490</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K90" s="6">
+        <v>31292</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>43920</v>
       </c>
@@ -2008,8 +2133,11 @@
       <c r="J91" s="5">
         <v>3466</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K91" s="6">
+        <v>31776</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>43921</v>
       </c>
@@ -2040,8 +2168,11 @@
       <c r="J92" s="5">
         <v>4070</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K92" s="6">
+        <v>32215</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>43922</v>
       </c>
@@ -2072,8 +2203,11 @@
       <c r="J93" s="5">
         <v>4530</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K93" s="6">
+        <v>32438</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>43923</v>
       </c>
@@ -2104,8 +2238,11 @@
       <c r="J94" s="5">
         <v>3834</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K94" s="6">
+        <v>32593</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>43924</v>
       </c>
@@ -2136,8 +2273,11 @@
       <c r="J95" s="5">
         <v>3834</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K95" s="6">
+        <v>32809</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>43925</v>
       </c>
@@ -2168,8 +2308,11 @@
       <c r="J96" s="5">
         <v>2928</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K96" s="6">
+        <v>33004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>43926</v>
       </c>
@@ -2200,8 +2343,11 @@
       <c r="J97" s="5">
         <v>2389</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K97" s="6">
+        <v>32926</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>43927</v>
       </c>
@@ -2232,8 +2378,11 @@
       <c r="J98" s="5">
         <v>1917</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K98" s="6">
+        <v>32874</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>43928</v>
       </c>
@@ -2264,8 +2413,11 @@
       <c r="J99" s="5">
         <v>2009</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K99" s="6">
+        <v>32510</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>43929</v>
       </c>
@@ -2296,8 +2448,11 @@
       <c r="J100" s="5">
         <v>2849</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K100" s="6">
+        <v>32178</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>43930</v>
       </c>
@@ -2328,8 +2483,11 @@
       <c r="J101" s="5">
         <v>2823</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K101" s="6">
+        <v>32004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>43931</v>
       </c>
@@ -2360,8 +2518,11 @@
       <c r="J102" s="5">
         <v>2009</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K102" s="6">
+        <v>31739</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>43932</v>
       </c>
@@ -2392,8 +2553,11 @@
       <c r="J103" s="5">
         <v>2061</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K103" s="6">
+        <v>31525</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>43933</v>
       </c>
@@ -2424,8 +2588,11 @@
       <c r="J104" s="5">
         <v>2035</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K104" s="6">
+        <v>31190</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>43934</v>
       </c>
@@ -2456,8 +2623,11 @@
       <c r="J105" s="5">
         <v>1234</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K105" s="6">
+        <v>31283</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>43935</v>
       </c>
@@ -2488,8 +2658,11 @@
       <c r="J106" s="5">
         <v>2074</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K106" s="6">
+        <v>31197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>43936</v>
       </c>
@@ -2520,8 +2693,11 @@
       <c r="J107" s="5">
         <v>1615</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K107" s="6">
+        <v>30722</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>43937</v>
       </c>
@@ -2552,8 +2728,11 @@
       <c r="J108" s="5">
         <v>1904</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K108" s="6">
+        <v>29829</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>43938</v>
       </c>
@@ -2584,8 +2763,11 @@
       <c r="J109" s="5">
         <v>2061</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K109" s="6">
+        <v>28598</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>43939</v>
       </c>
@@ -2616,8 +2798,11 @@
       <c r="J110" s="5">
         <v>1208</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K110" s="6">
+        <v>27740</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>43940</v>
       </c>
@@ -2648,8 +2833,11 @@
       <c r="J111" s="5">
         <v>867</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K111" s="6">
+        <v>27668</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>43941</v>
       </c>
@@ -2680,8 +2868,11 @@
       <c r="J112" s="5">
         <v>1037</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K112" s="6">
+        <v>27479</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>43942</v>
       </c>
@@ -2712,8 +2903,11 @@
       <c r="J113" s="5">
         <v>1103</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K113" s="6">
+        <v>26605</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>43943</v>
       </c>
@@ -2744,8 +2938,11 @@
       <c r="J114" s="5">
         <v>1103</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K114" s="6">
+        <v>26189</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>43944</v>
       </c>
@@ -2776,8 +2973,11 @@
       <c r="J115" s="5">
         <v>1129</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K115" s="6">
+        <v>25138</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>43945</v>
       </c>
@@ -2808,8 +3008,11 @@
       <c r="J116" s="5">
         <v>893</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K116" s="6">
+        <v>24241</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>43946</v>
       </c>
@@ -2840,8 +3043,11 @@
       <c r="J117" s="5">
         <v>1786</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K117" s="6">
+        <v>23635</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>43947</v>
       </c>
@@ -2872,8 +3078,11 @@
       <c r="J118" s="5">
         <v>473</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K118" s="6">
+        <v>23381</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>43948</v>
       </c>
@@ -2904,8 +3113,11 @@
       <c r="J119" s="5">
         <v>775</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K119" s="6">
+        <v>22309</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>43949</v>
       </c>
@@ -2936,8 +3148,11 @@
       <c r="J120" s="5">
         <v>1103</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K120" s="6">
+        <v>21586</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>43950</v>
       </c>
@@ -2968,8 +3183,11 @@
       <c r="J121" s="5">
         <v>814</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K121" s="6">
+        <v>21005</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>43951</v>
       </c>
@@ -3000,8 +3218,11 @@
       <c r="J122" s="5">
         <v>709</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K122" s="6">
+        <v>19843</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>43952</v>
       </c>
@@ -3032,8 +3253,11 @@
       <c r="J123" s="5">
         <v>538</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K123" s="6">
+        <v>19147</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>43953</v>
       </c>
@@ -3064,8 +3288,11 @@
       <c r="J124" s="5">
         <v>538</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K124" s="6">
+        <v>18896</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>43954</v>
       </c>
@@ -3096,8 +3323,11 @@
       <c r="J125" s="5">
         <v>394</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K125" s="6">
+        <v>18743</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>43955</v>
       </c>
@@ -3128,8 +3358,11 @@
       <c r="J126" s="5">
         <v>709</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K126" s="6">
+        <v>18302</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>43956</v>
       </c>
@@ -3160,8 +3393,11 @@
       <c r="J127" s="5">
         <v>840</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K127" s="6">
+        <v>17697</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>43957</v>
       </c>
@@ -3192,8 +3428,11 @@
       <c r="J128" s="5">
         <v>525</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K128" s="6">
+        <v>17102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>43958</v>
       </c>
@@ -3224,8 +3463,11 @@
       <c r="J129" s="5">
         <v>748</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K129" s="6">
+        <v>16485</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>43959</v>
       </c>
@@ -3256,8 +3498,11 @@
       <c r="J130" s="5">
         <v>473</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K130" s="6">
+        <v>15804</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>43960</v>
       </c>
@@ -3288,8 +3533,11 @@
       <c r="J131" s="5">
         <v>433</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K131" s="6">
+        <v>14868</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>43961</v>
       </c>
@@ -3320,8 +3568,11 @@
       <c r="J132" s="5">
         <v>263</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K132" s="6">
+        <v>14645</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>43962</v>
       </c>
@@ -3352,8 +3603,11 @@
       <c r="J133" s="5">
         <v>499</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K133" s="6">
+        <v>14538</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>43963</v>
       </c>
@@ -3384,8 +3638,11 @@
       <c r="J134" s="5">
         <v>407</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K134" s="6">
+        <v>13817</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>43964</v>
       </c>
@@ -3416,8 +3673,11 @@
       <c r="J135" s="5">
         <v>315</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K135" s="6">
+        <v>13065</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>43965</v>
       </c>
@@ -3448,8 +3708,11 @@
       <c r="J136" s="5">
         <v>263</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K136" s="6">
+        <v>12308</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>43966</v>
       </c>
@@ -3480,8 +3743,11 @@
       <c r="J137" s="5">
         <v>236</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K137" s="6">
+        <v>11600</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>43967</v>
       </c>
@@ -3512,8 +3778,11 @@
       <c r="J138" s="5">
         <v>276</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K138" s="6">
+        <v>11175</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>43968</v>
       </c>
@@ -3544,8 +3813,11 @@
       <c r="J139" s="5">
         <v>158</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K139" s="6">
+        <v>11073</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>43969</v>
       </c>
@@ -3576,8 +3848,11 @@
       <c r="J140" s="5">
         <v>171</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K140" s="6">
+        <v>10956</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>43970</v>
       </c>
@@ -3608,8 +3883,11 @@
       <c r="J141" s="5">
         <v>197</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K141" s="6">
+        <v>10707</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>43971</v>
       </c>
@@ -3640,8 +3918,11 @@
       <c r="J142" s="5">
         <v>144</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K142" s="6">
+        <v>10300</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>43972</v>
       </c>
@@ -3672,8 +3953,11 @@
       <c r="J143" s="5">
         <v>118</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K143" s="6">
+        <v>9909</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>43973</v>
       </c>
@@ -3704,8 +3988,11 @@
       <c r="J144" s="5">
         <v>118</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K144" s="6">
+        <v>9552</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>43974</v>
       </c>
@@ -3736,8 +4023,11 @@
       <c r="J145" s="5">
         <v>79</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K145" s="6">
+        <v>9267</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>43975</v>
       </c>
@@ -3765,8 +4055,11 @@
       <c r="I146" s="4">
         <v>589</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K146" s="6">
+        <v>9166</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>43976</v>
       </c>
@@ -3794,8 +4087,11 @@
       <c r="I147" s="4">
         <v>683</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K147" s="6">
+        <v>8726</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>43977</v>
       </c>
@@ -3823,8 +4119,11 @@
       <c r="I148" s="4">
         <v>707</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K148" s="6">
+        <v>8438</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>43978</v>
       </c>
@@ -3852,8 +4151,11 @@
       <c r="I149" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K149" s="6">
+        <v>8234</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>43979</v>
       </c>
@@ -3881,8 +4183,11 @@
       <c r="I150" s="4">
         <v>631</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K150" s="6">
+        <v>7868</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>43980</v>
       </c>
@@ -3910,8 +4215,11 @@
       <c r="I151" s="4">
         <v>580</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K151" s="6">
+        <v>7569</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>43981</v>
       </c>
@@ -3939,8 +4247,11 @@
       <c r="I152" s="4">
         <v>548</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K152" s="6">
+        <v>7130</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>43982</v>
       </c>
@@ -3968,8 +4279,11 @@
       <c r="I153" s="4">
         <v>604</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K153" s="6">
+        <v>6822</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>43983</v>
       </c>
@@ -3997,8 +4311,11 @@
       <c r="I154" s="4">
         <v>635</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K154" s="6">
+        <v>6523</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>43984</v>
       </c>
@@ -4026,8 +4343,11 @@
       <c r="I155" s="4">
         <v>605</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K155" s="6">
+        <v>6324</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>43985</v>
       </c>
@@ -4055,8 +4375,11 @@
       <c r="I156" s="4">
         <v>599</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K156" s="6">
+        <v>6095</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>43986</v>
       </c>
@@ -4084,8 +4407,11 @@
       <c r="I157" s="4">
         <v>486</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K157" s="6">
+        <v>5841</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>43987</v>
       </c>
@@ -4113,8 +4439,11 @@
       <c r="I158" s="4">
         <v>400</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K158" s="6">
+        <v>5617</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>43988</v>
       </c>
@@ -4142,8 +4471,11 @@
       <c r="I159" s="4">
         <v>423</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K159" s="6">
+        <v>5295</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>43989</v>
       </c>
@@ -4171,8 +4503,11 @@
       <c r="I160" s="4">
         <v>431</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K160" s="6">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>43990</v>
       </c>
@@ -4200,8 +4535,11 @@
       <c r="I161" s="4">
         <v>461</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K161" s="6">
+        <v>5012</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>43991</v>
       </c>
@@ -4229,8 +4567,11 @@
       <c r="I162" s="4">
         <v>497</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K162" s="6">
+        <v>4844</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>43992</v>
       </c>
@@ -4258,8 +4599,11 @@
       <c r="I163" s="4">
         <v>440</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K163" s="6">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>43993</v>
       </c>
@@ -4287,8 +4631,11 @@
       <c r="I164" s="4">
         <v>413</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K164" s="6">
+        <v>4367</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>43994</v>
       </c>
@@ -4316,8 +4663,11 @@
       <c r="I165" s="4">
         <v>358</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K165" s="6">
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>43995</v>
       </c>
@@ -4345,8 +4695,11 @@
       <c r="I166" s="4">
         <v>426</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K166" s="6">
+        <v>3967</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>43996</v>
       </c>
@@ -4374,8 +4727,11 @@
       <c r="I167" s="4">
         <v>423</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K167" s="6">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>43997</v>
       </c>
@@ -4403,8 +4759,11 @@
       <c r="I168" s="4">
         <v>428</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K168" s="6">
+        <v>3696</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>43998</v>
       </c>
@@ -4432,8 +4791,11 @@
       <c r="I169" s="4">
         <v>434</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K169" s="6">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>43999</v>
       </c>
@@ -4461,8 +4823,11 @@
       <c r="I170" s="4">
         <v>409</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K170" s="6">
+        <v>3276</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>44000</v>
       </c>
@@ -4490,8 +4855,11 @@
       <c r="I171" s="4">
         <v>342</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K171" s="6">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>44001</v>
       </c>
@@ -4519,8 +4887,11 @@
       <c r="I172" s="4">
         <v>266</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K172" s="6">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>44002</v>
       </c>
@@ -4548,8 +4919,11 @@
       <c r="I173" s="4">
         <v>288</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K173" s="6">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>44003</v>
       </c>
@@ -4577,8 +4951,11 @@
       <c r="I174" s="4">
         <v>390</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K174" s="6">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>44004</v>
       </c>
@@ -4606,8 +4983,11 @@
       <c r="I175" s="4">
         <v>347</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K175" s="6">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>44005</v>
       </c>
@@ -4635,8 +5015,11 @@
       <c r="I176" s="4">
         <v>347</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K176" s="6">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>44006</v>
       </c>
@@ -4664,8 +5047,11 @@
       <c r="I177" s="4">
         <v>361</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K177" s="6">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>44007</v>
       </c>
@@ -4693,8 +5079,11 @@
       <c r="I178" s="4">
         <v>315</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K178" s="6">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>44008</v>
       </c>
@@ -4722,8 +5111,11 @@
       <c r="I179" s="4">
         <v>298</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K179" s="6">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>44009</v>
       </c>
@@ -4751,8 +5143,11 @@
       <c r="I180" s="4">
         <v>231</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K180" s="6">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>44010</v>
       </c>
@@ -4780,8 +5175,11 @@
       <c r="I181" s="4">
         <v>224</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K181" s="6">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>44011</v>
       </c>
@@ -4809,8 +5207,11 @@
       <c r="I182" s="4">
         <v>237</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K182" s="6">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>44012</v>
       </c>
@@ -4838,8 +5239,11 @@
       <c r="I183" s="4">
         <v>306</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K183" s="6">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>44013</v>
       </c>
@@ -4867,8 +5271,11 @@
       <c r="I184" s="4">
         <v>217</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K184" s="6">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>44014</v>
       </c>
@@ -4896,8 +5303,11 @@
       <c r="I185" s="4">
         <v>210</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K185" s="6">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>44015</v>
       </c>
@@ -4925,8 +5335,11 @@
       <c r="I186" s="4">
         <v>187</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K186" s="6">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>44016</v>
       </c>
@@ -4954,8 +5367,11 @@
       <c r="I187" s="4">
         <v>212</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K187" s="6">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>44017</v>
       </c>
@@ -4983,8 +5399,11 @@
       <c r="I188" s="4">
         <v>215</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K188" s="6">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>44018</v>
       </c>
@@ -5012,8 +5431,11 @@
       <c r="I189" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K189" s="6">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>44019</v>
       </c>
@@ -5041,8 +5463,11 @@
       <c r="I190" s="4">
         <v>206</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K190" s="6">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>44020</v>
       </c>
@@ -5070,8 +5495,11 @@
       <c r="I191" s="4">
         <v>201</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K191" s="6">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>44021</v>
       </c>
@@ -5099,8 +5527,11 @@
       <c r="I192" s="4">
         <v>179</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K192" s="6">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>44022</v>
       </c>
@@ -5128,8 +5559,11 @@
       <c r="I193" s="4">
         <v>167</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K193" s="6">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>44023</v>
       </c>
@@ -5157,8 +5591,11 @@
       <c r="I194" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K194" s="6">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>44024</v>
       </c>
@@ -5186,8 +5623,11 @@
       <c r="I195" s="4">
         <v>179</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K195" s="6">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>44025</v>
       </c>
@@ -5215,8 +5655,11 @@
       <c r="I196" s="4">
         <v>173</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K196" s="6">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>44026</v>
       </c>
@@ -5244,8 +5687,11 @@
       <c r="I197" s="4">
         <v>179</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K197" s="6">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>44027</v>
       </c>
@@ -5273,8 +5719,11 @@
       <c r="I198" s="4">
         <v>163</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K198" s="6">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>44028</v>
       </c>
@@ -5299,8 +5748,11 @@
       <c r="H199" s="4">
         <v>1690</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K199" s="6">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>44029</v>
       </c>
@@ -5325,8 +5777,11 @@
       <c r="H200" s="4">
         <v>1676</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K200" s="6">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>44030</v>
       </c>
@@ -5351,8 +5806,11 @@
       <c r="H201" s="4">
         <v>1649</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K201" s="6">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>44031</v>
       </c>
@@ -5377,8 +5835,11 @@
       <c r="H202" s="4">
         <v>1613</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K202" s="6">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>44032</v>
       </c>
@@ -5403,8 +5864,11 @@
       <c r="H203" s="4">
         <v>1600</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K203" s="6">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>44033</v>
       </c>
@@ -5429,8 +5893,11 @@
       <c r="H204" s="4">
         <v>1510</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K204" s="6">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>44034</v>
       </c>
@@ -5455,8 +5922,11 @@
       <c r="H205" s="4">
         <v>1637</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K205" s="6">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>44035</v>
       </c>
@@ -5481,8 +5951,11 @@
       <c r="H206" s="4">
         <v>1445</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K206" s="6">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>44036</v>
       </c>
@@ -5507,8 +5980,11 @@
       <c r="H207" s="4">
         <v>1346</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K207" s="6">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>44037</v>
       </c>
@@ -5533,8 +6009,11 @@
       <c r="H208" s="4">
         <v>1257</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K208" s="6">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>44038</v>
       </c>
@@ -5559,8 +6038,11 @@
       <c r="H209" s="4">
         <v>1286</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K209" s="6">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>44039</v>
       </c>
@@ -5582,8 +6064,11 @@
       <c r="G210" s="3">
         <v>118</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K210" s="6">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>44040</v>
       </c>
@@ -5596,13 +6081,19 @@
       <c r="G211" s="3">
         <v>172</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K211" s="6">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>44041</v>
       </c>
       <c r="B212">
         <v>211</v>
+      </c>
+      <c r="K212" s="6">
+        <v>769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Push ICU data Sweden
</commit_message>
<xml_diff>
--- a/data/hospitalisation_data/hospital_data_europe.xlsx
+++ b/data/hospitalisation_data/hospital_data_europe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\data\hospitalisation_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4865A293-F0E8-4910-ABE1-7455CF22C27D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8B7A6E-4F04-4331-91F6-07850B86637A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>data</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>italy_hospital_occupancy</t>
+  </si>
+  <si>
+    <t>sweden_icu_admission</t>
   </si>
 </sst>
 </file>
@@ -935,28 +938,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K212"/>
+  <dimension ref="A1:L212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I165" sqref="I165"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L209" sqref="L209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.08984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32.81640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="32.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,8 +994,11 @@
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -999,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43832</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>43833</v>
       </c>
@@ -1015,7 +1022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>43834</v>
       </c>
@@ -1023,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>43835</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>43836</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>43837</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43838</v>
       </c>
@@ -1055,7 +1062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>43839</v>
       </c>
@@ -1063,7 +1070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>43840</v>
       </c>
@@ -1071,7 +1078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>43841</v>
       </c>
@@ -1079,7 +1086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>43842</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>43843</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>43844</v>
       </c>
@@ -1103,7 +1110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>43845</v>
       </c>
@@ -1522,7 +1529,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>43894</v>
       </c>
@@ -1533,7 +1540,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43895</v>
       </c>
@@ -1544,7 +1551,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>43896</v>
       </c>
@@ -1554,8 +1561,11 @@
       <c r="K67" s="6">
         <v>2856</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>43897</v>
       </c>
@@ -1565,8 +1575,11 @@
       <c r="K68" s="6">
         <v>3218</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>43898</v>
       </c>
@@ -1576,8 +1589,11 @@
       <c r="K69" s="6">
         <v>4207</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>43899</v>
       </c>
@@ -1587,8 +1603,11 @@
       <c r="K70" s="6">
         <v>5049</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>43900</v>
       </c>
@@ -1601,8 +1620,11 @@
       <c r="K71" s="6">
         <v>5915</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L71" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>43901</v>
       </c>
@@ -1615,8 +1637,11 @@
       <c r="K72" s="6">
         <v>6866</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>43902</v>
       </c>
@@ -1629,8 +1654,11 @@
       <c r="K73" s="6">
         <v>7803</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L73" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>43903</v>
       </c>
@@ -1643,8 +1671,11 @@
       <c r="K74" s="6">
         <v>8754</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L74" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>43904</v>
       </c>
@@ -1657,8 +1688,11 @@
       <c r="K75" s="6">
         <v>9890</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L75" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>43905</v>
       </c>
@@ -1680,8 +1714,11 @@
       <c r="K76" s="6">
         <v>11335</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L76" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>43906</v>
       </c>
@@ -1703,8 +1740,11 @@
       <c r="K77" s="6">
         <v>12876</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L77" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>43907</v>
       </c>
@@ -1726,8 +1766,11 @@
       <c r="K78" s="6">
         <v>14954</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L78" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>43908</v>
       </c>
@@ -1752,8 +1795,11 @@
       <c r="K79" s="6">
         <v>16620</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L79" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>43909</v>
       </c>
@@ -1781,8 +1827,11 @@
       <c r="K80" s="6">
         <v>18255</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L80" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>43910</v>
       </c>
@@ -1810,8 +1859,11 @@
       <c r="K81" s="6">
         <v>18675</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L81" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>43911</v>
       </c>
@@ -1839,8 +1891,11 @@
       <c r="K82" s="6">
         <v>20565</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L82" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>43912</v>
       </c>
@@ -1868,8 +1923,11 @@
       <c r="K83" s="6">
         <v>22855</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L83" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>43913</v>
       </c>
@@ -1900,8 +1958,11 @@
       <c r="K84" s="6">
         <v>23896</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L84" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>43914</v>
       </c>
@@ -1932,8 +1993,11 @@
       <c r="K85" s="6">
         <v>25333</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L85" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>43915</v>
       </c>
@@ -1964,8 +2028,11 @@
       <c r="K86" s="6">
         <v>26601</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L86" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>43916</v>
       </c>
@@ -1996,8 +2063,11 @@
       <c r="K87" s="6">
         <v>28365</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L87" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>43917</v>
       </c>
@@ -2031,8 +2101,11 @@
       <c r="K88" s="6">
         <v>29761</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L88" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>43918</v>
       </c>
@@ -2066,8 +2139,11 @@
       <c r="K89" s="6">
         <v>30532</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L89" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>43919</v>
       </c>
@@ -2101,8 +2177,11 @@
       <c r="K90" s="6">
         <v>31292</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L90" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>43920</v>
       </c>
@@ -2136,8 +2215,11 @@
       <c r="K91" s="6">
         <v>31776</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L91" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>43921</v>
       </c>
@@ -2171,8 +2253,11 @@
       <c r="K92" s="6">
         <v>32215</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L92" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>43922</v>
       </c>
@@ -2206,8 +2291,11 @@
       <c r="K93" s="6">
         <v>32438</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L93" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>43923</v>
       </c>
@@ -2241,8 +2329,11 @@
       <c r="K94" s="6">
         <v>32593</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L94" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>43924</v>
       </c>
@@ -2276,8 +2367,11 @@
       <c r="K95" s="6">
         <v>32809</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L95" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>43925</v>
       </c>
@@ -2311,8 +2405,11 @@
       <c r="K96" s="6">
         <v>33004</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L96" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>43926</v>
       </c>
@@ -2346,8 +2443,11 @@
       <c r="K97" s="6">
         <v>32926</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L97" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>43927</v>
       </c>
@@ -2381,8 +2481,11 @@
       <c r="K98" s="6">
         <v>32874</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L98" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>43928</v>
       </c>
@@ -2416,8 +2519,11 @@
       <c r="K99" s="6">
         <v>32510</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L99" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>43929</v>
       </c>
@@ -2451,8 +2557,11 @@
       <c r="K100" s="6">
         <v>32178</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L100" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>43930</v>
       </c>
@@ -2486,8 +2595,11 @@
       <c r="K101" s="6">
         <v>32004</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L101" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>43931</v>
       </c>
@@ -2521,8 +2633,11 @@
       <c r="K102" s="6">
         <v>31739</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L102" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>43932</v>
       </c>
@@ -2556,8 +2671,11 @@
       <c r="K103" s="6">
         <v>31525</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L103" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>43933</v>
       </c>
@@ -2591,8 +2709,11 @@
       <c r="K104" s="6">
         <v>31190</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L104" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>43934</v>
       </c>
@@ -2626,8 +2747,11 @@
       <c r="K105" s="6">
         <v>31283</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L105" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>43935</v>
       </c>
@@ -2661,8 +2785,11 @@
       <c r="K106" s="6">
         <v>31197</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L106" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>43936</v>
       </c>
@@ -2696,8 +2823,11 @@
       <c r="K107" s="6">
         <v>30722</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L107" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>43937</v>
       </c>
@@ -2731,8 +2861,11 @@
       <c r="K108" s="6">
         <v>29829</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L108" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>43938</v>
       </c>
@@ -2766,8 +2899,11 @@
       <c r="K109" s="6">
         <v>28598</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L109" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>43939</v>
       </c>
@@ -2801,8 +2937,11 @@
       <c r="K110" s="6">
         <v>27740</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L110" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>43940</v>
       </c>
@@ -2836,8 +2975,11 @@
       <c r="K111" s="6">
         <v>27668</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L111" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>43941</v>
       </c>
@@ -2871,8 +3013,11 @@
       <c r="K112" s="6">
         <v>27479</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L112" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>43942</v>
       </c>
@@ -2906,8 +3051,11 @@
       <c r="K113" s="6">
         <v>26605</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L113" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>43943</v>
       </c>
@@ -2941,8 +3089,11 @@
       <c r="K114" s="6">
         <v>26189</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L114" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>43944</v>
       </c>
@@ -2976,8 +3127,11 @@
       <c r="K115" s="6">
         <v>25138</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L115" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>43945</v>
       </c>
@@ -3011,8 +3165,11 @@
       <c r="K116" s="6">
         <v>24241</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L116" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>43946</v>
       </c>
@@ -3046,8 +3203,11 @@
       <c r="K117" s="6">
         <v>23635</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L117" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>43947</v>
       </c>
@@ -3081,8 +3241,11 @@
       <c r="K118" s="6">
         <v>23381</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L118" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>43948</v>
       </c>
@@ -3116,8 +3279,11 @@
       <c r="K119" s="6">
         <v>22309</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L119" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>43949</v>
       </c>
@@ -3151,8 +3317,11 @@
       <c r="K120" s="6">
         <v>21586</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L120" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>43950</v>
       </c>
@@ -3186,8 +3355,11 @@
       <c r="K121" s="6">
         <v>21005</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L121" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>43951</v>
       </c>
@@ -3221,8 +3393,11 @@
       <c r="K122" s="6">
         <v>19843</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L122" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>43952</v>
       </c>
@@ -3256,8 +3431,11 @@
       <c r="K123" s="6">
         <v>19147</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L123" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>43953</v>
       </c>
@@ -3291,8 +3469,11 @@
       <c r="K124" s="6">
         <v>18896</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L124" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>43954</v>
       </c>
@@ -3326,8 +3507,11 @@
       <c r="K125" s="6">
         <v>18743</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L125" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>43955</v>
       </c>
@@ -3361,8 +3545,11 @@
       <c r="K126" s="6">
         <v>18302</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L126" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>43956</v>
       </c>
@@ -3396,8 +3583,11 @@
       <c r="K127" s="6">
         <v>17697</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L127" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>43957</v>
       </c>
@@ -3431,8 +3621,11 @@
       <c r="K128" s="6">
         <v>17102</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L128" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>43958</v>
       </c>
@@ -3466,8 +3659,11 @@
       <c r="K129" s="6">
         <v>16485</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L129" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>43959</v>
       </c>
@@ -3501,8 +3697,11 @@
       <c r="K130" s="6">
         <v>15804</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L130" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>43960</v>
       </c>
@@ -3536,8 +3735,11 @@
       <c r="K131" s="6">
         <v>14868</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L131" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>43961</v>
       </c>
@@ -3571,8 +3773,11 @@
       <c r="K132" s="6">
         <v>14645</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L132" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>43962</v>
       </c>
@@ -3606,8 +3811,11 @@
       <c r="K133" s="6">
         <v>14538</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L133" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>43963</v>
       </c>
@@ -3641,8 +3849,11 @@
       <c r="K134" s="6">
         <v>13817</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L134" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>43964</v>
       </c>
@@ -3676,8 +3887,11 @@
       <c r="K135" s="6">
         <v>13065</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L135" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>43965</v>
       </c>
@@ -3711,8 +3925,11 @@
       <c r="K136" s="6">
         <v>12308</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L136" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>43966</v>
       </c>
@@ -3746,8 +3963,11 @@
       <c r="K137" s="6">
         <v>11600</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L137" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>43967</v>
       </c>
@@ -3781,8 +4001,11 @@
       <c r="K138" s="6">
         <v>11175</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L138" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>43968</v>
       </c>
@@ -3816,8 +4039,11 @@
       <c r="K139" s="6">
         <v>11073</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L139" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>43969</v>
       </c>
@@ -3851,8 +4077,11 @@
       <c r="K140" s="6">
         <v>10956</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L140" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>43970</v>
       </c>
@@ -3886,8 +4115,11 @@
       <c r="K141" s="6">
         <v>10707</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L141" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>43971</v>
       </c>
@@ -3921,8 +4153,11 @@
       <c r="K142" s="6">
         <v>10300</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L142" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>43972</v>
       </c>
@@ -3956,8 +4191,11 @@
       <c r="K143" s="6">
         <v>9909</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L143" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>43973</v>
       </c>
@@ -3991,8 +4229,11 @@
       <c r="K144" s="6">
         <v>9552</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L144" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>43974</v>
       </c>
@@ -4026,8 +4267,11 @@
       <c r="K145" s="6">
         <v>9267</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L145" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>43975</v>
       </c>
@@ -4058,8 +4302,11 @@
       <c r="K146" s="6">
         <v>9166</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L146" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>43976</v>
       </c>
@@ -4090,8 +4337,11 @@
       <c r="K147" s="6">
         <v>8726</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L147" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>43977</v>
       </c>
@@ -4122,8 +4372,11 @@
       <c r="K148" s="6">
         <v>8438</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L148" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>43978</v>
       </c>
@@ -4154,8 +4407,11 @@
       <c r="K149" s="6">
         <v>8234</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L149" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>43979</v>
       </c>
@@ -4186,8 +4442,11 @@
       <c r="K150" s="6">
         <v>7868</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L150" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>43980</v>
       </c>
@@ -4218,8 +4477,11 @@
       <c r="K151" s="6">
         <v>7569</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L151" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>43981</v>
       </c>
@@ -4250,8 +4512,11 @@
       <c r="K152" s="6">
         <v>7130</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L152" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>43982</v>
       </c>
@@ -4282,8 +4547,11 @@
       <c r="K153" s="6">
         <v>6822</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L153" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>43983</v>
       </c>
@@ -4314,8 +4582,11 @@
       <c r="K154" s="6">
         <v>6523</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L154" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>43984</v>
       </c>
@@ -4346,8 +4617,11 @@
       <c r="K155" s="6">
         <v>6324</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L155" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>43985</v>
       </c>
@@ -4378,8 +4652,11 @@
       <c r="K156" s="6">
         <v>6095</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L156" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>43986</v>
       </c>
@@ -4410,8 +4687,11 @@
       <c r="K157" s="6">
         <v>5841</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L157" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>43987</v>
       </c>
@@ -4442,8 +4722,11 @@
       <c r="K158" s="6">
         <v>5617</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L158" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>43988</v>
       </c>
@@ -4474,8 +4757,11 @@
       <c r="K159" s="6">
         <v>5295</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L159" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>43989</v>
       </c>
@@ -4506,8 +4792,11 @@
       <c r="K160" s="6">
         <v>5151</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L160" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>43990</v>
       </c>
@@ -4538,8 +4827,11 @@
       <c r="K161" s="6">
         <v>5012</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L161" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>43991</v>
       </c>
@@ -4570,8 +4862,11 @@
       <c r="K162" s="6">
         <v>4844</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L162" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>43992</v>
       </c>
@@ -4602,8 +4897,11 @@
       <c r="K163" s="6">
         <v>4569</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L163" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>43993</v>
       </c>
@@ -4634,8 +4932,11 @@
       <c r="K164" s="6">
         <v>4367</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L164" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>43994</v>
       </c>
@@ -4666,8 +4967,11 @@
       <c r="K165" s="6">
         <v>4120</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L165" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>43995</v>
       </c>
@@ -4698,8 +5002,11 @@
       <c r="K166" s="6">
         <v>3967</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L166" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>43996</v>
       </c>
@@ -4730,8 +5037,11 @@
       <c r="K167" s="6">
         <v>3803</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L167" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>43997</v>
       </c>
@@ -4762,8 +5072,11 @@
       <c r="K168" s="6">
         <v>3696</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L168" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>43998</v>
       </c>
@@ -4794,8 +5107,11 @@
       <c r="K169" s="6">
         <v>3478</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L169" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>43999</v>
       </c>
@@ -4826,8 +5142,11 @@
       <c r="K170" s="6">
         <v>3276</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L170" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>44000</v>
       </c>
@@ -4858,8 +5177,11 @@
       <c r="K171" s="6">
         <v>3035</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L171" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>44001</v>
       </c>
@@ -4890,8 +5212,11 @@
       <c r="K172" s="6">
         <v>2793</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L172" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>44002</v>
       </c>
@@ -4922,8 +5247,11 @@
       <c r="K173" s="6">
         <v>2626</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L173" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>44003</v>
       </c>
@@ -4954,8 +5282,11 @@
       <c r="K174" s="6">
         <v>2462</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L174" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>44004</v>
       </c>
@@ -4986,8 +5317,11 @@
       <c r="K175" s="6">
         <v>2165</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L175" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>44005</v>
       </c>
@@ -5018,8 +5352,11 @@
       <c r="K176" s="6">
         <v>1968</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L176" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>44006</v>
       </c>
@@ -5050,8 +5387,11 @@
       <c r="K177" s="6">
         <v>1717</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L177" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>44007</v>
       </c>
@@ -5082,8 +5422,11 @@
       <c r="K178" s="6">
         <v>1618</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L178" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>44008</v>
       </c>
@@ -5114,8 +5457,11 @@
       <c r="K179" s="6">
         <v>1461</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L179" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>44009</v>
       </c>
@@ -5146,8 +5492,11 @@
       <c r="K180" s="6">
         <v>1357</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L180" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>44010</v>
       </c>
@@ -5178,8 +5527,11 @@
       <c r="K181" s="6">
         <v>1258</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L181" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>44011</v>
       </c>
@@ -5210,8 +5562,11 @@
       <c r="K182" s="6">
         <v>1216</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L182" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>44012</v>
       </c>
@@ -5242,8 +5597,11 @@
       <c r="K183" s="6">
         <v>1183</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L183" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>44013</v>
       </c>
@@ -5274,8 +5632,11 @@
       <c r="K184" s="6">
         <v>1112</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L184" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>44014</v>
       </c>
@@ -5306,8 +5667,11 @@
       <c r="K185" s="6">
         <v>1045</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L185" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>44015</v>
       </c>
@@ -5338,8 +5702,11 @@
       <c r="K186" s="6">
         <v>1035</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L186" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>44016</v>
       </c>
@@ -5370,8 +5737,11 @@
       <c r="K187" s="6">
         <v>1011</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L187" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>44017</v>
       </c>
@@ -5402,8 +5772,11 @@
       <c r="K188" s="6">
         <v>1019</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L188" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>44018</v>
       </c>
@@ -5434,8 +5807,11 @@
       <c r="K189" s="6">
         <v>1018</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L189" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>44019</v>
       </c>
@@ -5466,8 +5842,11 @@
       <c r="K190" s="6">
         <v>1010</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L190" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>44020</v>
       </c>
@@ -5498,8 +5877,11 @@
       <c r="K191" s="6">
         <v>970</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L191" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>44021</v>
       </c>
@@ -5530,8 +5912,11 @@
       <c r="K192" s="6">
         <v>940</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L192" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>44022</v>
       </c>
@@ -5562,8 +5947,11 @@
       <c r="K193" s="6">
         <v>909</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L193" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>44023</v>
       </c>
@@ -5594,8 +5982,11 @@
       <c r="K194" s="6">
         <v>893</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L194" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>44024</v>
       </c>
@@ -5626,8 +6017,11 @@
       <c r="K195" s="6">
         <v>844</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L195" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>44025</v>
       </c>
@@ -5658,8 +6052,11 @@
       <c r="K196" s="6">
         <v>833</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L196" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>44026</v>
       </c>
@@ -5690,8 +6087,11 @@
       <c r="K197" s="6">
         <v>837</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L197" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>44027</v>
       </c>
@@ -5722,8 +6122,11 @@
       <c r="K198" s="6">
         <v>854</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L198" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>44028</v>
       </c>
@@ -5751,8 +6154,11 @@
       <c r="K199" s="6">
         <v>803</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L199" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>44029</v>
       </c>
@@ -5780,8 +6186,11 @@
       <c r="K200" s="6">
         <v>821</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L200" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>44030</v>
       </c>
@@ -5809,8 +6218,11 @@
       <c r="K201" s="6">
         <v>807</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L201" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>44031</v>
       </c>
@@ -5838,8 +6250,11 @@
       <c r="K202" s="6">
         <v>792</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L202" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>44032</v>
       </c>
@@ -5867,8 +6282,11 @@
       <c r="K203" s="6">
         <v>792</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L203" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>44033</v>
       </c>
@@ -5896,8 +6314,11 @@
       <c r="K204" s="6">
         <v>781</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L204" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>44034</v>
       </c>
@@ -5925,8 +6346,11 @@
       <c r="K205" s="6">
         <v>772</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L205" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>44035</v>
       </c>
@@ -5954,8 +6378,11 @@
       <c r="K206" s="6">
         <v>762</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L206" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>44036</v>
       </c>
@@ -5984,7 +6411,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>44037</v>
       </c>

</xml_diff>